<commit_message>
add img src and update
</commit_message>
<xml_diff>
--- a/docs/pages/tools/weapon_table_maker/excel/d_ナックル.xlsx
+++ b/docs/pages/tools/weapon_table_maker/excel/d_ナックル.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyle\Desktop\wepons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyle\Desktop\git_repository\PSNOVA\docs\pages\tools\weapon_table_maker\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0532517-C26C-429A-9D50-DD0BCF701E80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F633ADEF-C04B-4176-A8DD-7BD3CE59053A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5895" yWindow="2370" windowWidth="20880" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="-120" windowWidth="28080" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="168">
   <si>
     <t>ナックル</t>
   </si>
@@ -42,9 +42,6 @@
     <t>白い岩石x1</t>
   </si>
   <si>
-    <t>アルバナックル</t>
-  </si>
-  <si>
     <t>02★2</t>
   </si>
   <si>
@@ -441,11 +438,97 @@
     <t>備考</t>
   </si>
   <si>
-    <t>基礎打撃力</t>
-    <rPh sb="2" eb="4">
-      <t>ダゲキ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
+    <t>打撃力</t>
+  </si>
+  <si>
+    <t>射撃力</t>
+  </si>
+  <si>
+    <t>法撃力</t>
+  </si>
+  <si>
+    <t>ショップLv</t>
+  </si>
+  <si>
+    <t>サボテン</t>
+  </si>
+  <si>
+    <t>イーグマンドーグ</t>
+  </si>
+  <si>
+    <t>13★13</t>
+  </si>
+  <si>
+    <t>ディゴルドスの極コアx1</t>
+  </si>
+  <si>
+    <t>イーグマンデルの超双角x3</t>
+  </si>
+  <si>
+    <t>エルマフレザールの極爪x3</t>
+  </si>
+  <si>
+    <t>マラカイトx3</t>
+  </si>
+  <si>
+    <t>グレイック</t>
+  </si>
+  <si>
+    <t>14★14</t>
+  </si>
+  <si>
+    <t>グレイオスの極コアx1</t>
+  </si>
+  <si>
+    <t>グレイオスの極背びれx3</t>
+  </si>
+  <si>
+    <t>アグリオスの極背びれx4</t>
+  </si>
+  <si>
+    <t>Gミクダの極甲羅x3</t>
+  </si>
+  <si>
+    <t>ジルコンx3</t>
+  </si>
+  <si>
+    <t>ノヴァクローグ</t>
+  </si>
+  <si>
+    <t>15★15</t>
+  </si>
+  <si>
+    <t>ヴァリゴルドスの極コア×1</t>
+  </si>
+  <si>
+    <t>ノヴァファクター×1</t>
+  </si>
+  <si>
+    <t>レイヴガイストの極結界×4</t>
+  </si>
+  <si>
+    <t>サブクランプの極巻き貝×3</t>
+  </si>
+  <si>
+    <t>真紅のルビー×3</t>
+  </si>
+  <si>
+    <t>ファイバーロア</t>
+  </si>
+  <si>
+    <t>ヴィヴリュードの極コアx1</t>
+  </si>
+  <si>
+    <t>ブラックチケットx3</t>
+  </si>
+  <si>
+    <t>アルレイバンサーの極銃x3</t>
+  </si>
+  <si>
+    <t>ギガティオンの極蹄x3</t>
+  </si>
+  <si>
+    <t>漆黒のオブシディアンx3</t>
   </si>
 </sst>
 </file>
@@ -770,32 +853,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:H125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" t="s">
         <v>134</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" t="s">
         <v>135</v>
       </c>
-      <c r="C1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>136</v>
       </c>
-      <c r="E1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -805,771 +897,968 @@
       <c r="C2">
         <v>105</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="D3" t="s">
+    <row r="3" spans="1:8">
+      <c r="G3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="D4" t="s">
+    <row r="4" spans="1:8">
+      <c r="G4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5">
+        <v>325</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="G6" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
-        <v>278</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="D6" t="s">
+    </row>
+    <row r="7" spans="1:8">
+      <c r="G7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>325</v>
-      </c>
-      <c r="D8" t="s">
+        <v>560</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>794</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>883</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="G17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="G18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>972</v>
+      </c>
+      <c r="F19">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11">
-        <v>560</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14">
-        <v>794</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="D16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="D17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
+      <c r="G19" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18">
-        <v>883</v>
-      </c>
-      <c r="D18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="D19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="D20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="D21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
+      <c r="H19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="G20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="G21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="G22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
         <v>24</v>
       </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22">
-        <v>972</v>
-      </c>
-      <c r="D22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="D23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="D24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="D25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
+      <c r="C23">
+        <v>1039</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23" t="s">
         <v>30</v>
       </c>
-      <c r="B26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26">
-        <v>1039</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="H23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="G24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="D27" t="s">
+    <row r="25" spans="1:8">
+      <c r="G25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="D28" t="s">
+    <row r="26" spans="1:8">
+      <c r="G26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
-      <c r="D29" t="s">
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="s">
+      <c r="B27" t="s">
         <v>35</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C27">
+        <v>1186</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="G27" t="s">
         <v>36</v>
       </c>
-      <c r="C30">
-        <v>1186</v>
-      </c>
-      <c r="D30" t="s">
+    </row>
+    <row r="28" spans="1:8">
+      <c r="G28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="D31" t="s">
+    <row r="29" spans="1:8">
+      <c r="G29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
-      <c r="D32" t="s">
+    <row r="30" spans="1:8">
+      <c r="G30" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="D33" t="s">
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31">
+        <v>1141</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31" t="s">
         <v>41</v>
       </c>
-      <c r="B34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34">
-        <v>1141</v>
-      </c>
-      <c r="D34" t="s">
+    </row>
+    <row r="32" spans="1:8">
+      <c r="G32" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="D35" t="s">
+    <row r="33" spans="1:7">
+      <c r="G33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="D36" t="s">
+    <row r="34" spans="1:7">
+      <c r="G34" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="D37" t="s">
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
+      <c r="B35" t="s">
         <v>46</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C35">
+        <v>1308</v>
+      </c>
+      <c r="F35">
+        <v>3</v>
+      </c>
+      <c r="G35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="G36" t="s">
         <v>47</v>
       </c>
-      <c r="C38">
-        <v>1308</v>
-      </c>
-      <c r="D38" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="D39" t="s">
+    </row>
+    <row r="37" spans="1:7">
+      <c r="G37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="G38" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="D40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="D41" t="s">
+    <row r="39" spans="1:7">
+      <c r="G39" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="D42" t="s">
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" t="s">
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40">
+        <v>1461</v>
+      </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+      <c r="G40" t="s">
         <v>51</v>
       </c>
-      <c r="B43" t="s">
-        <v>47</v>
-      </c>
-      <c r="C43">
-        <v>1461</v>
-      </c>
-      <c r="D43" t="s">
+    </row>
+    <row r="41" spans="1:7">
+      <c r="G41" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="D44" t="s">
+    <row r="42" spans="1:7">
+      <c r="G42" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="D45" t="s">
+    <row r="43" spans="1:7">
+      <c r="G43" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="D46" t="s">
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" t="s">
+      <c r="B44" t="s">
         <v>56</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C44">
+        <v>1615</v>
+      </c>
+      <c r="F44">
+        <v>3</v>
+      </c>
+      <c r="G44" t="s">
         <v>57</v>
       </c>
-      <c r="C47">
-        <v>1615</v>
-      </c>
-      <c r="D47" t="s">
+    </row>
+    <row r="45" spans="1:7">
+      <c r="G45" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="D48" t="s">
+    <row r="46" spans="1:7">
+      <c r="G46" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="D49" t="s">
+    <row r="47" spans="1:7">
+      <c r="G47" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="D50" t="s">
+    <row r="48" spans="1:7">
+      <c r="G48" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="D51" t="s">
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" t="s">
+      <c r="B49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49">
+        <v>1678</v>
+      </c>
+      <c r="F49">
+        <v>3</v>
+      </c>
+      <c r="G49" t="s">
         <v>63</v>
       </c>
-      <c r="B52" t="s">
-        <v>57</v>
-      </c>
-      <c r="C52">
-        <v>1678</v>
-      </c>
-      <c r="D52" t="s">
+    </row>
+    <row r="50" spans="1:7">
+      <c r="G50" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="D53" t="s">
+    <row r="51" spans="1:7">
+      <c r="G51" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="D54" t="s">
+    <row r="52" spans="1:7">
+      <c r="G52" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
-      <c r="D55" t="s">
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
+      <c r="B53" t="s">
         <v>68</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C53">
+        <v>1962</v>
+      </c>
+      <c r="F53">
+        <v>3</v>
+      </c>
+      <c r="G53" t="s">
         <v>69</v>
       </c>
-      <c r="C56">
-        <v>1962</v>
-      </c>
-      <c r="D56" t="s">
+    </row>
+    <row r="54" spans="1:7">
+      <c r="G54" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
-      <c r="D57" t="s">
+    <row r="55" spans="1:7">
+      <c r="G55" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="G56" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
-      <c r="D58" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="D59" t="s">
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" t="s">
+      <c r="B57" t="s">
+        <v>68</v>
+      </c>
+      <c r="C57">
+        <v>1865</v>
+      </c>
+      <c r="F57">
+        <v>3</v>
+      </c>
+      <c r="G57" t="s">
         <v>73</v>
       </c>
-      <c r="B60" t="s">
-        <v>69</v>
-      </c>
-      <c r="C60">
-        <v>1865</v>
-      </c>
-      <c r="D60" t="s">
+    </row>
+    <row r="58" spans="1:7">
+      <c r="G58" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
-      <c r="D61" t="s">
+    <row r="59" spans="1:7">
+      <c r="G59" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
-      <c r="D62" t="s">
+    <row r="60" spans="1:7">
+      <c r="G60" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
-      <c r="D63" t="s">
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" t="s">
+      <c r="B61" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61">
+        <v>1821</v>
+      </c>
+      <c r="F61">
+        <v>3</v>
+      </c>
+      <c r="G61" t="s">
         <v>78</v>
       </c>
-      <c r="B64" t="s">
-        <v>69</v>
-      </c>
-      <c r="C64">
-        <v>1821</v>
-      </c>
-      <c r="D64" t="s">
+    </row>
+    <row r="62" spans="1:7">
+      <c r="G62" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
-      <c r="D65" t="s">
+    <row r="63" spans="1:7">
+      <c r="G63" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
-      <c r="D66" t="s">
+    <row r="64" spans="1:7">
+      <c r="G64" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
-      <c r="D67" t="s">
+    <row r="65" spans="1:7">
+      <c r="A65" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" t="s">
+      <c r="B65" t="s">
         <v>83</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C65">
+        <v>2026</v>
+      </c>
+      <c r="F65">
+        <v>4</v>
+      </c>
+      <c r="G65" t="s">
         <v>84</v>
       </c>
-      <c r="C68">
-        <v>2026</v>
-      </c>
-      <c r="D68" t="s">
+    </row>
+    <row r="66" spans="1:7">
+      <c r="G66" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
-      <c r="D69" t="s">
+    <row r="67" spans="1:7">
+      <c r="G67" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
-      <c r="D70" t="s">
+    <row r="68" spans="1:7">
+      <c r="G68" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
-      <c r="D71" t="s">
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" t="s">
+      <c r="B69" t="s">
+        <v>83</v>
+      </c>
+      <c r="C69">
+        <v>2179</v>
+      </c>
+      <c r="F69">
+        <v>4</v>
+      </c>
+      <c r="G69" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="G70" t="s">
         <v>89</v>
       </c>
-      <c r="B72" t="s">
-        <v>84</v>
-      </c>
-      <c r="C72">
-        <v>2179</v>
-      </c>
-      <c r="D72" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="D73" t="s">
+    </row>
+    <row r="71" spans="1:7">
+      <c r="G71" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="G72" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
-      <c r="D74" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="D75" t="s">
+    <row r="73" spans="1:7">
+      <c r="A73" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" t="s">
+      <c r="B73" t="s">
+        <v>83</v>
+      </c>
+      <c r="C73">
+        <v>2313</v>
+      </c>
+      <c r="F73">
+        <v>4</v>
+      </c>
+      <c r="G73" t="s">
         <v>92</v>
       </c>
-      <c r="B76" t="s">
-        <v>84</v>
-      </c>
-      <c r="C76">
-        <v>2313</v>
-      </c>
-      <c r="D76" t="s">
+    </row>
+    <row r="74" spans="1:7">
+      <c r="G74" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
-      <c r="D77" t="s">
+    <row r="75" spans="1:7">
+      <c r="G75" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="G76" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
-      <c r="D78" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="D79" t="s">
+    <row r="77" spans="1:7">
+      <c r="G77" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
-      <c r="D80" t="s">
+    <row r="78" spans="1:7">
+      <c r="A78" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" t="s">
+      <c r="B78" t="s">
         <v>97</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C78">
+        <v>2770</v>
+      </c>
+      <c r="F78">
+        <v>5</v>
+      </c>
+      <c r="G78" t="s">
         <v>98</v>
       </c>
-      <c r="C81">
+    </row>
+    <row r="79" spans="1:7">
+      <c r="G79" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="G80" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="G81" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" t="s">
+        <v>102</v>
+      </c>
+      <c r="B82" t="s">
+        <v>97</v>
+      </c>
+      <c r="C82">
         <v>2770</v>
       </c>
-      <c r="D81" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="D82" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="D83" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="D84" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
-      <c r="A85" t="s">
+      <c r="F82">
+        <v>5</v>
+      </c>
+      <c r="G82" t="s">
         <v>103</v>
       </c>
-      <c r="B85" t="s">
-        <v>98</v>
-      </c>
-      <c r="C85">
+    </row>
+    <row r="83" spans="1:7">
+      <c r="G83" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="G84" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="G85" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="G86" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" t="s">
+        <v>108</v>
+      </c>
+      <c r="B87" t="s">
+        <v>97</v>
+      </c>
+      <c r="C87">
         <v>2770</v>
       </c>
-      <c r="D85" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
-      <c r="D86" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4">
-      <c r="D87" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="D88" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="D89" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="A90" t="s">
+      <c r="F87">
+        <v>5</v>
+      </c>
+      <c r="G87" t="s">
         <v>109</v>
       </c>
-      <c r="B90" t="s">
-        <v>98</v>
-      </c>
-      <c r="C90">
+    </row>
+    <row r="88" spans="1:7">
+      <c r="G88" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="G89" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="G90" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="G91" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" t="s">
+        <v>114</v>
+      </c>
+      <c r="B92" t="s">
+        <v>97</v>
+      </c>
+      <c r="C92">
         <v>2770</v>
       </c>
-      <c r="D90" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
-      <c r="D91" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="D92" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="D93" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="D94" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
-      <c r="A95" t="s">
+      <c r="F92">
+        <v>5</v>
+      </c>
+      <c r="G92" t="s">
         <v>115</v>
       </c>
-      <c r="B95" t="s">
-        <v>98</v>
-      </c>
-      <c r="C95">
-        <v>2770</v>
-      </c>
-      <c r="D95" t="s">
+    </row>
+    <row r="93" spans="1:7">
+      <c r="G93" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
-      <c r="D96" t="s">
+    <row r="94" spans="1:7">
+      <c r="G94" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
-      <c r="D97" t="s">
+    <row r="95" spans="1:7">
+      <c r="G95" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
-      <c r="D98" t="s">
+    <row r="96" spans="1:7">
+      <c r="G96" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
-      <c r="D99" t="s">
+    <row r="97" spans="1:7">
+      <c r="A97" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="100" spans="1:4">
-      <c r="A100" t="s">
+      <c r="B97" t="s">
         <v>121</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C97">
+        <v>3181</v>
+      </c>
+      <c r="F97">
+        <v>5</v>
+      </c>
+      <c r="G97" t="s">
         <v>122</v>
       </c>
-      <c r="C100">
-        <v>3181</v>
-      </c>
-      <c r="D100" t="s">
+    </row>
+    <row r="98" spans="1:7">
+      <c r="G98" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
-      <c r="D101" t="s">
+    <row r="99" spans="1:7">
+      <c r="G99" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
-      <c r="D102" t="s">
+    <row r="100" spans="1:7">
+      <c r="G100" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
-      <c r="D103" t="s">
+    <row r="101" spans="1:7">
+      <c r="G101" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
-      <c r="D104" t="s">
+    <row r="102" spans="1:7">
+      <c r="A102" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="105" spans="1:4">
-      <c r="A105" t="s">
+      <c r="B102" t="s">
+        <v>121</v>
+      </c>
+      <c r="C102">
+        <v>3500</v>
+      </c>
+      <c r="F102">
+        <v>5</v>
+      </c>
+      <c r="G102" t="s">
         <v>128</v>
       </c>
-      <c r="B105" t="s">
-        <v>122</v>
-      </c>
-      <c r="C105">
-        <v>3500</v>
-      </c>
-      <c r="D105" t="s">
+    </row>
+    <row r="103" spans="1:7">
+      <c r="G103" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
-      <c r="D106" t="s">
+    <row r="104" spans="1:7">
+      <c r="G104" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
-      <c r="D107" t="s">
+    <row r="105" spans="1:7">
+      <c r="G105" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
-      <c r="D108" t="s">
+    <row r="106" spans="1:7">
+      <c r="G106" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
-      <c r="D109" t="s">
-        <v>133</v>
+    <row r="107" spans="1:7">
+      <c r="A107" t="s">
+        <v>142</v>
+      </c>
+      <c r="B107" t="s">
+        <v>143</v>
+      </c>
+      <c r="C107">
+        <v>4013</v>
+      </c>
+      <c r="F107">
+        <v>5</v>
+      </c>
+      <c r="G107" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="G108" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="G109" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="G110" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" t="s">
+        <v>148</v>
+      </c>
+      <c r="B111" t="s">
+        <v>149</v>
+      </c>
+      <c r="C111">
+        <v>4618</v>
+      </c>
+      <c r="F111">
+        <v>5</v>
+      </c>
+      <c r="G111" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="G112" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="G113" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="G114" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="G115" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
+      <c r="A116" t="s">
+        <v>155</v>
+      </c>
+      <c r="B116" t="s">
+        <v>156</v>
+      </c>
+      <c r="C116">
+        <v>9019</v>
+      </c>
+      <c r="F116">
+        <v>5</v>
+      </c>
+      <c r="G116" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
+      <c r="G117" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
+      <c r="G118" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
+      <c r="G119" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="G120" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" t="s">
+        <v>162</v>
+      </c>
+      <c r="B121" t="s">
+        <v>156</v>
+      </c>
+      <c r="C121">
+        <v>5920</v>
+      </c>
+      <c r="F121">
+        <v>5</v>
+      </c>
+      <c r="G121" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="G122" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="G123" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="G124" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
+      <c r="G125" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>